<commit_message>
Update PLANILLA DE EVALUACIÓN FASE 3 - PRESENTACION FINAL.xlsx
</commit_message>
<xml_diff>
--- a/fase 3/Evidencias Grupales/PLANILLA DE EVALUACIÓN FASE 3 - PRESENTACION FINAL.xlsx
+++ b/fase 3/Evidencias Grupales/PLANILLA DE EVALUACIÓN FASE 3 - PRESENTACION FINAL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29602"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://duoccl0-my.sharepoint.com/personal/ge_galan_profesor_duoc_cl/Documents/2024-2/Clases/CAPSTONE/DOCUMENTOS FASE3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="777" documentId="8_{2EFDF332-31E9-4C74-A6B5-E695634C1C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DA9E333-109C-40E4-9CB6-8C2D20BED8EE}"/>
+  <xr:revisionPtr revIDLastSave="928" documentId="8_{2EFDF332-31E9-4C74-A6B5-E695634C1C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D93CE2E-1000-4C78-88DB-05459F5F8A60}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="65">
   <si>
     <t>INTEGRANTES</t>
   </si>
@@ -80,13 +80,10 @@
     <t>Nota final</t>
   </si>
   <si>
-    <t>ESTUDIANTE 1</t>
+    <t>CHRISTOPH BORNHARDT</t>
   </si>
   <si>
-    <t>ESTUDIANTE 2</t>
-  </si>
-  <si>
-    <t>ESTUDIANTE 3</t>
+    <t>JOAN JARA</t>
   </si>
   <si>
     <t>DOCENTE</t>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>Nota</t>
+  </si>
+  <si>
+    <t>Logro incipiente</t>
   </si>
   <si>
     <t>COMISION 1</t>
@@ -283,9 +283,6 @@
   </si>
   <si>
     <t>Relevancia</t>
-  </si>
-  <si>
-    <t>Logro incipiente</t>
   </si>
   <si>
     <t>Muy Relevante</t>
@@ -830,7 +827,10 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -842,7 +842,7 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -875,9 +875,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1212,7 +1209,7 @@
   <dimension ref="A2:K797"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A50" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelRow="1"/>
@@ -1263,15 +1260,15 @@
       </c>
       <c r="C4" s="31">
         <f>C21</f>
-        <v>7</v>
+        <v>4.8</v>
       </c>
       <c r="D4" s="37">
         <f>C60</f>
-        <v>7</v>
+        <v>4.8</v>
       </c>
       <c r="E4" s="36">
         <f>C4*C$2+D4*D$2</f>
-        <v>7</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="14.45">
@@ -1283,84 +1280,82 @@
       </c>
       <c r="C5" s="31">
         <f>C34</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D5" s="37">
         <f>C73</f>
-        <v>7</v>
+        <v>4.2</v>
       </c>
       <c r="E5" s="36">
         <f t="shared" ref="E5:E6" si="0">C5*C$2+D5*D$2</f>
-        <v>7</v>
+        <v>4.0599999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="14.45">
       <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>6</v>
-      </c>
+      <c r="B6" s="16"/>
       <c r="C6" s="31">
         <f>C47</f>
-        <v>7</v>
+        <v>5.2</v>
       </c>
       <c r="D6" s="37">
         <f>C86</f>
-        <v>7</v>
+        <v>5.2</v>
       </c>
       <c r="E6" s="36">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5.1999999999999993</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="18" outlineLevel="1">
-      <c r="A11" s="38" t="s">
-        <v>7</v>
+      <c r="A11" s="43" t="s">
+        <v>6</v>
       </c>
       <c r="B11" s="11" t="str">
         <f>B4</f>
-        <v>ESTUDIANTE 1</v>
-      </c>
-      <c r="C11" s="39" t="s">
+        <v>CHRISTOPH BORNHARDT</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="53"/>
+    </row>
+    <row r="12" spans="1:11" ht="14.45" outlineLevel="1">
+      <c r="A12" s="54"/>
+      <c r="B12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="52"/>
-    </row>
-    <row r="12" spans="1:11" ht="14.45" outlineLevel="1">
-      <c r="A12" s="53"/>
-      <c r="B12" s="15" t="s">
+      <c r="C12" s="55"/>
+      <c r="D12" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="54"/>
-      <c r="D12" s="40" t="s">
+      <c r="E12" s="53"/>
+      <c r="F12" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="52"/>
-      <c r="F12" s="40" t="s">
+      <c r="G12" s="53"/>
+      <c r="H12" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="52"/>
-      <c r="H12" s="41" t="s">
+      <c r="I12" s="53"/>
+      <c r="J12" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="52"/>
-      <c r="J12" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="52"/>
+      <c r="K12" s="53"/>
     </row>
     <row r="13" spans="1:11" ht="24" outlineLevel="1">
-      <c r="A13" s="55"/>
+      <c r="A13" s="56"/>
       <c r="B13" s="19" t="str">
         <f>RUBRICA!A4</f>
         <v xml:space="preserve">1. Presenta el proyecto considerando la relevancia, objetivos, metodología y desarrollo, de acuerdo a los estándares de calidad de la disciplina. </v>
@@ -1370,19 +1365,19 @@
       </c>
       <c r="D13" s="12" t="str">
         <f t="shared" ref="D13:D17" si="1">IF($C13=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E13" s="12">
+        <v/>
+      </c>
+      <c r="E13" s="12" t="str">
         <f>IF(D13="X",100*0.15,"")</f>
-        <v>15</v>
+        <v/>
       </c>
       <c r="F13" s="12" t="str">
         <f t="shared" ref="F13:F17" si="2">IF($C13=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G13" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G13" s="12">
         <f>IF(F13="X",60*0.15,"")</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="H13" s="12" t="str">
         <f t="shared" ref="H13:H17" si="3">IF($C13=ML,"X","")</f>
@@ -1402,7 +1397,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="26.45" customHeight="1" outlineLevel="1">
-      <c r="A14" s="55"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="19" t="str">
         <f>RUBRICA!A5</f>
         <v xml:space="preserve">2. Presenta las evidencias del Proyecto APT, dando cuenta del cumplimiento de los objetivos y de acuerdo a los estándares de la disciplina. </v>
@@ -1412,19 +1407,19 @@
       </c>
       <c r="D14" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="E14" s="12">
+        <v/>
+      </c>
+      <c r="E14" s="12" t="str">
         <f>IF(D14="X",100*0.25,"")</f>
-        <v>25</v>
+        <v/>
       </c>
       <c r="F14" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G14" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G14" s="12">
         <f>IF(F14="X",60*0.25,"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="H14" s="12" t="str">
         <f t="shared" si="3"/>
@@ -1444,7 +1439,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="24" outlineLevel="1">
-      <c r="A15" s="55"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="19" t="str">
         <f>RUBRICA!A6</f>
         <v>3. Responde las preguntas realizadas por la comisión, cumpliendo con los estándares de calidad de la disciplina.</v>
@@ -1454,19 +1449,19 @@
       </c>
       <c r="D15" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="E15" s="12">
+        <v/>
+      </c>
+      <c r="E15" s="12" t="str">
         <f>IF(D15="X",100*0.2,"")</f>
-        <v>20</v>
+        <v/>
       </c>
       <c r="F15" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G15" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G15" s="12">
         <f>IF(F15="X",60*0.2,"")</f>
-        <v/>
+        <v>12</v>
       </c>
       <c r="H15" s="12" t="str">
         <f t="shared" si="3"/>
@@ -1486,13 +1481,13 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="24" outlineLevel="1">
-      <c r="A16" s="55"/>
+      <c r="A16" s="56"/>
       <c r="B16" s="19" t="str">
         <f>RUBRICA!A7</f>
         <v>4. Expone el Proyecto APT, considerando el formato y el tiempo establecido para la presentación.</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" s="12" t="str">
         <f t="shared" si="1"/>
@@ -1528,7 +1523,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="24" outlineLevel="1">
-      <c r="A17" s="55"/>
+      <c r="A17" s="56"/>
       <c r="B17" s="19" t="str">
         <f>RUBRICA!A8</f>
         <v>5. Expresa sus ideas con fluidez, claridad y precisión, utilizando lenguaje técnico propio de la disciplina.</v>
@@ -1538,19 +1533,19 @@
       </c>
       <c r="D17" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="E17" s="12">
+        <v/>
+      </c>
+      <c r="E17" s="12" t="str">
         <f>IF(D17="X",100*0.05,"")</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="F17" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G17" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G17" s="12">
         <f>IF(F17="X",60*0.05,"")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="H17" s="12" t="str">
         <f t="shared" si="3"/>
@@ -1570,13 +1565,13 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="24" outlineLevel="1">
-      <c r="A18" s="55"/>
+      <c r="A18" s="56"/>
       <c r="B18" s="19" t="str">
         <f>RUBRICA!A9</f>
         <v>6. Entrega la documentación y evidencias requerida por la asignatura de acuerdo a la estructura y nombres solicitados, guardando todas las evidencias de avances en Git</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D18" s="12" t="str">
         <f>IF($C18=CL,"X","")</f>
@@ -1612,7 +1607,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="24" outlineLevel="1">
-      <c r="A19" s="55"/>
+      <c r="A19" s="56"/>
       <c r="B19" s="19" t="str">
         <f>RUBRICA!A10</f>
         <v xml:space="preserve">7. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. </v>
@@ -1622,19 +1617,19 @@
       </c>
       <c r="D19" s="12" t="str">
         <f>IF($C19=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E19" s="12">
+        <v/>
+      </c>
+      <c r="E19" s="12" t="str">
         <f>IF(D19="X",100*0.1,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F19" s="12" t="str">
         <f>IF($C19=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G19" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G19" s="12">
         <f>IF(F19="X",60*0.1,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="H19" s="12" t="str">
         <f>IF($C19=ML,"X","")</f>
@@ -1654,23 +1649,23 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1">
-      <c r="A20" s="53"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="22">
         <f>E20+G20+I20+K20</f>
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="13">
         <f>SUM(E13:E19)</f>
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="13">
         <f>SUM(G13:G19)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="H20" s="13"/>
       <c r="I20" s="13">
@@ -1684,64 +1679,64 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1">
-      <c r="A21" s="54"/>
+      <c r="A21" s="55"/>
       <c r="B21" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="14">
         <f>VLOOKUP(C20,ESCALA_IEP!A2:B202,2,FALSE)</f>
-        <v>7</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1"/>
     <row r="23" spans="1:11" ht="15.75" customHeight="1"/>
     <row r="24" spans="1:11" ht="24" customHeight="1">
-      <c r="A24" s="38" t="s">
-        <v>7</v>
+      <c r="A24" s="43" t="s">
+        <v>6</v>
       </c>
       <c r="B24" s="11" t="str">
         <f>B5</f>
-        <v>ESTUDIANTE 2</v>
-      </c>
-      <c r="C24" s="39" t="s">
+        <v>JOAN JARA</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="40" t="s">
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="53"/>
+    </row>
+    <row r="25" spans="1:11" ht="24" customHeight="1">
+      <c r="A25" s="54"/>
+      <c r="B25" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="51"/>
-      <c r="I24" s="51"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="52"/>
-    </row>
-    <row r="25" spans="1:11" ht="24" customHeight="1">
-      <c r="A25" s="53"/>
-      <c r="B25" s="15" t="s">
+      <c r="C25" s="55"/>
+      <c r="D25" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="40" t="s">
+      <c r="E25" s="53"/>
+      <c r="F25" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="52"/>
-      <c r="F25" s="40" t="s">
+      <c r="G25" s="53"/>
+      <c r="H25" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="52"/>
-      <c r="H25" s="41" t="s">
+      <c r="I25" s="53"/>
+      <c r="J25" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="I25" s="52"/>
-      <c r="J25" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="K25" s="52"/>
+      <c r="K25" s="53"/>
     </row>
     <row r="26" spans="1:11" ht="24" customHeight="1">
-      <c r="A26" s="55"/>
+      <c r="A26" s="56"/>
       <c r="B26" s="19" t="str">
         <f>RUBRICA!A4</f>
         <v xml:space="preserve">1. Presenta el proyecto considerando la relevancia, objetivos, metodología y desarrollo, de acuerdo a los estándares de calidad de la disciplina. </v>
@@ -1751,19 +1746,19 @@
       </c>
       <c r="D26" s="12" t="str">
         <f t="shared" ref="D26:D30" si="7">IF($C26=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E26" s="12">
+        <v/>
+      </c>
+      <c r="E26" s="12" t="str">
         <f>IF(D26="X",100*0.15,"")</f>
-        <v>15</v>
+        <v/>
       </c>
       <c r="F26" s="12" t="str">
         <f t="shared" ref="F26:F30" si="8">IF($C26=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G26" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G26" s="12">
         <f>IF(F26="X",60*0.15,"")</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="H26" s="12" t="str">
         <f t="shared" ref="H26:H30" si="9">IF($C26=ML,"X","")</f>
@@ -1783,7 +1778,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="24" customHeight="1">
-      <c r="A27" s="55"/>
+      <c r="A27" s="56"/>
       <c r="B27" s="19" t="str">
         <f>RUBRICA!A5</f>
         <v xml:space="preserve">2. Presenta las evidencias del Proyecto APT, dando cuenta del cumplimiento de los objetivos y de acuerdo a los estándares de la disciplina. </v>
@@ -1793,19 +1788,19 @@
       </c>
       <c r="D27" s="12" t="str">
         <f t="shared" si="7"/>
-        <v>X</v>
-      </c>
-      <c r="E27" s="12">
+        <v/>
+      </c>
+      <c r="E27" s="12" t="str">
         <f>IF(D27="X",100*0.25,"")</f>
-        <v>25</v>
+        <v/>
       </c>
       <c r="F27" s="12" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G27" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G27" s="12">
         <f>IF(F27="X",60*0.25,"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="H27" s="12" t="str">
         <f t="shared" si="9"/>
@@ -1825,21 +1820,21 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="24" customHeight="1">
-      <c r="A28" s="55"/>
+      <c r="A28" s="56"/>
       <c r="B28" s="19" t="str">
         <f>RUBRICA!A6</f>
         <v>3. Responde las preguntas realizadas por la comisión, cumpliendo con los estándares de calidad de la disciplina.</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D28" s="12" t="str">
         <f t="shared" si="7"/>
-        <v>X</v>
-      </c>
-      <c r="E28" s="12">
+        <v/>
+      </c>
+      <c r="E28" s="12" t="str">
         <f>IF(D28="X",100*0.2,"")</f>
-        <v>20</v>
+        <v/>
       </c>
       <c r="F28" s="12" t="str">
         <f t="shared" si="8"/>
@@ -1851,11 +1846,11 @@
       </c>
       <c r="H28" s="12" t="str">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="I28" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="I28" s="12">
         <f>IF(H28="X",30*0.2,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="J28" s="12" t="str">
         <f t="shared" si="10"/>
@@ -1867,13 +1862,13 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="24" customHeight="1">
-      <c r="A29" s="55"/>
+      <c r="A29" s="56"/>
       <c r="B29" s="19" t="str">
         <f>RUBRICA!A7</f>
         <v>4. Expone el Proyecto APT, considerando el formato y el tiempo establecido para la presentación.</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D29" s="12" t="str">
         <f t="shared" si="7"/>
@@ -1909,21 +1904,21 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="24" customHeight="1">
-      <c r="A30" s="55"/>
+      <c r="A30" s="56"/>
       <c r="B30" s="19" t="str">
         <f>RUBRICA!A8</f>
         <v>5. Expresa sus ideas con fluidez, claridad y precisión, utilizando lenguaje técnico propio de la disciplina.</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D30" s="12" t="str">
         <f t="shared" si="7"/>
-        <v>X</v>
-      </c>
-      <c r="E30" s="12">
+        <v/>
+      </c>
+      <c r="E30" s="12" t="str">
         <f>IF(D30="X",100*0.05,"")</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="F30" s="12" t="str">
         <f t="shared" si="8"/>
@@ -1935,11 +1930,11 @@
       </c>
       <c r="H30" s="12" t="str">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="I30" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="I30" s="12">
         <f>IF(H30="X",30*0.05,"")</f>
-        <v/>
+        <v>1.5</v>
       </c>
       <c r="J30" s="12" t="str">
         <f t="shared" si="10"/>
@@ -1951,13 +1946,13 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="24" customHeight="1">
-      <c r="A31" s="55"/>
+      <c r="A31" s="56"/>
       <c r="B31" s="19" t="str">
         <f>RUBRICA!A9</f>
         <v>6. Entrega la documentación y evidencias requerida por la asignatura de acuerdo a la estructura y nombres solicitados, guardando todas las evidencias de avances en Git</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D31" s="12" t="str">
         <f>IF($C31=CL,"X","")</f>
@@ -1993,21 +1988,21 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="24" customHeight="1">
-      <c r="A32" s="55"/>
+      <c r="A32" s="56"/>
       <c r="B32" s="19" t="str">
         <f>RUBRICA!A10</f>
         <v xml:space="preserve">7. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. </v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D32" s="12" t="str">
         <f>IF($C32=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E32" s="12">
+        <v/>
+      </c>
+      <c r="E32" s="12" t="str">
         <f>IF(D32="X",100*0.1,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F32" s="12" t="str">
         <f>IF($C32=L,"X","")</f>
@@ -2019,11 +2014,11 @@
       </c>
       <c r="H32" s="12" t="str">
         <f>IF($C32=ML,"X","")</f>
-        <v/>
-      </c>
-      <c r="I32" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="I32" s="12">
         <f>IF(H32="X",30*0.1,"")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="J32" s="12" t="str">
         <f>IF($C32=NL,"X","")</f>
@@ -2035,28 +2030,28 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="24" customHeight="1">
-      <c r="A33" s="53"/>
+      <c r="A33" s="54"/>
       <c r="B33" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33" s="22">
         <f>E33+G33+I33+K33</f>
-        <v>100</v>
+        <v>59.5</v>
       </c>
       <c r="D33" s="13"/>
       <c r="E33" s="13">
         <f>SUM(E26:E32)</f>
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F33" s="13"/>
       <c r="G33" s="13">
         <f>SUM(G26:G32)</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="H33" s="13"/>
       <c r="I33" s="13">
         <f>SUM(I26:I32)</f>
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="J33" s="13"/>
       <c r="K33" s="13">
@@ -2065,70 +2060,70 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="24" customHeight="1">
-      <c r="A34" s="54"/>
+      <c r="A34" s="55"/>
       <c r="B34" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C34" s="14">
         <f>VLOOKUP(C33,ESCALA_IEP!A15:B215,2,FALSE)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="16.149999999999999" customHeight="1"/>
     <row r="36" spans="1:11" ht="13.9" customHeight="1"/>
     <row r="37" spans="1:11" ht="24" customHeight="1">
-      <c r="A37" s="38" t="s">
+      <c r="A37" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="11">
+        <f>B6</f>
+        <v>0</v>
+      </c>
+      <c r="C37" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="11" t="str">
-        <f>B6</f>
-        <v>ESTUDIANTE 3</v>
-      </c>
-      <c r="C37" s="39" t="s">
+      <c r="D37" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="40" t="s">
+      <c r="E37" s="52"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="53"/>
+    </row>
+    <row r="38" spans="1:11" ht="24" customHeight="1">
+      <c r="A38" s="54"/>
+      <c r="B38" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E37" s="51"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="51"/>
-      <c r="H37" s="51"/>
-      <c r="I37" s="51"/>
-      <c r="J37" s="51"/>
-      <c r="K37" s="52"/>
-    </row>
-    <row r="38" spans="1:11" ht="24" customHeight="1">
-      <c r="A38" s="53"/>
-      <c r="B38" s="15" t="s">
+      <c r="C38" s="55"/>
+      <c r="D38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="54"/>
-      <c r="D38" s="40" t="s">
+      <c r="E38" s="53"/>
+      <c r="F38" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="52"/>
-      <c r="F38" s="40" t="s">
+      <c r="G38" s="53"/>
+      <c r="H38" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="G38" s="52"/>
-      <c r="H38" s="41" t="s">
+      <c r="I38" s="53"/>
+      <c r="J38" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="I38" s="52"/>
-      <c r="J38" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="K38" s="52"/>
+      <c r="K38" s="53"/>
     </row>
     <row r="39" spans="1:11" ht="24" customHeight="1">
-      <c r="A39" s="55"/>
+      <c r="A39" s="56"/>
       <c r="B39" s="19" t="str">
         <f>RUBRICA!A4</f>
         <v xml:space="preserve">1. Presenta el proyecto considerando la relevancia, objetivos, metodología y desarrollo, de acuerdo a los estándares de calidad de la disciplina. </v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D39" s="12" t="str">
         <f t="shared" ref="D39:D43" si="12">IF($C39=CL,"X","")</f>
@@ -2164,7 +2159,7 @@
       </c>
     </row>
     <row r="40" spans="1:11" ht="24" customHeight="1">
-      <c r="A40" s="55"/>
+      <c r="A40" s="56"/>
       <c r="B40" s="19" t="str">
         <f>RUBRICA!A5</f>
         <v xml:space="preserve">2. Presenta las evidencias del Proyecto APT, dando cuenta del cumplimiento de los objetivos y de acuerdo a los estándares de la disciplina. </v>
@@ -2174,19 +2169,19 @@
       </c>
       <c r="D40" s="12" t="str">
         <f t="shared" si="12"/>
-        <v>X</v>
-      </c>
-      <c r="E40" s="12">
+        <v/>
+      </c>
+      <c r="E40" s="12" t="str">
         <f>IF(D40="X",100*0.25,"")</f>
-        <v>25</v>
+        <v/>
       </c>
       <c r="F40" s="12" t="str">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="G40" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G40" s="12">
         <f>IF(F40="X",60*0.25,"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="H40" s="12" t="str">
         <f t="shared" si="14"/>
@@ -2206,7 +2201,7 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="24" customHeight="1">
-      <c r="A41" s="55"/>
+      <c r="A41" s="56"/>
       <c r="B41" s="19" t="str">
         <f>RUBRICA!A6</f>
         <v>3. Responde las preguntas realizadas por la comisión, cumpliendo con los estándares de calidad de la disciplina.</v>
@@ -2216,19 +2211,19 @@
       </c>
       <c r="D41" s="12" t="str">
         <f t="shared" si="12"/>
-        <v>X</v>
-      </c>
-      <c r="E41" s="12">
+        <v/>
+      </c>
+      <c r="E41" s="12" t="str">
         <f>IF(D41="X",100*0.2,"")</f>
-        <v>20</v>
+        <v/>
       </c>
       <c r="F41" s="12" t="str">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="G41" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G41" s="12">
         <f>IF(F41="X",60*0.2,"")</f>
-        <v/>
+        <v>12</v>
       </c>
       <c r="H41" s="12" t="str">
         <f t="shared" si="14"/>
@@ -2248,13 +2243,13 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="24" customHeight="1">
-      <c r="A42" s="55"/>
+      <c r="A42" s="56"/>
       <c r="B42" s="19" t="str">
         <f>RUBRICA!A7</f>
         <v>4. Expone el Proyecto APT, considerando el formato y el tiempo establecido para la presentación.</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D42" s="12" t="str">
         <f t="shared" si="12"/>
@@ -2290,7 +2285,7 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="24" customHeight="1">
-      <c r="A43" s="55"/>
+      <c r="A43" s="56"/>
       <c r="B43" s="19" t="str">
         <f>RUBRICA!A8</f>
         <v>5. Expresa sus ideas con fluidez, claridad y precisión, utilizando lenguaje técnico propio de la disciplina.</v>
@@ -2300,19 +2295,19 @@
       </c>
       <c r="D43" s="12" t="str">
         <f t="shared" si="12"/>
-        <v>X</v>
-      </c>
-      <c r="E43" s="12">
+        <v/>
+      </c>
+      <c r="E43" s="12" t="str">
         <f>IF(D43="X",100*0.05,"")</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="F43" s="12" t="str">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="G43" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G43" s="12">
         <f>IF(F43="X",60*0.05,"")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="H43" s="12" t="str">
         <f t="shared" si="14"/>
@@ -2332,13 +2327,13 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="24" customHeight="1">
-      <c r="A44" s="55"/>
+      <c r="A44" s="56"/>
       <c r="B44" s="19" t="str">
         <f>RUBRICA!A9</f>
         <v>6. Entrega la documentación y evidencias requerida por la asignatura de acuerdo a la estructura y nombres solicitados, guardando todas las evidencias de avances en Git</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D44" s="12" t="str">
         <f>IF($C44=CL,"X","")</f>
@@ -2374,7 +2369,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="24" customHeight="1">
-      <c r="A45" s="55"/>
+      <c r="A45" s="56"/>
       <c r="B45" s="19" t="str">
         <f>RUBRICA!A10</f>
         <v xml:space="preserve">7. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. </v>
@@ -2384,19 +2379,19 @@
       </c>
       <c r="D45" s="12" t="str">
         <f>IF($C45=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E45" s="12">
+        <v/>
+      </c>
+      <c r="E45" s="12" t="str">
         <f>IF(D45="X",100*0.1,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F45" s="12" t="str">
         <f>IF($C45=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G45" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G45" s="12">
         <f>IF(F45="X",60*0.1,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="H45" s="12" t="str">
         <f>IF($C45=ML,"X","")</f>
@@ -2416,23 +2411,23 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="24" customHeight="1">
-      <c r="A46" s="53"/>
+      <c r="A46" s="54"/>
       <c r="B46" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C46" s="22">
         <f>E46+G46+I46+K46</f>
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="D46" s="13"/>
       <c r="E46" s="13">
         <f>SUM(E39:E45)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="F46" s="13"/>
       <c r="G46" s="13">
         <f>SUM(G39:G45)</f>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="H46" s="13"/>
       <c r="I46" s="13">
@@ -2446,64 +2441,64 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="24" customHeight="1">
-      <c r="A47" s="54"/>
+      <c r="A47" s="55"/>
       <c r="B47" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C47" s="14">
         <f>VLOOKUP(C46,ESCALA_IEP!A28:B228,2,FALSE)</f>
-        <v>7</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1"/>
     <row r="49" spans="1:11" ht="15.75" customHeight="1"/>
     <row r="50" spans="1:11" ht="24" customHeight="1">
-      <c r="A50" s="42" t="s">
+      <c r="A50" s="39" t="s">
         <v>17</v>
       </c>
       <c r="B50" s="11" t="str">
         <f>B4</f>
-        <v>ESTUDIANTE 1</v>
-      </c>
-      <c r="C50" s="39" t="s">
+        <v>CHRISTOPH BORNHARDT</v>
+      </c>
+      <c r="C50" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D50" s="40" t="s">
+      <c r="E50" s="52"/>
+      <c r="F50" s="52"/>
+      <c r="G50" s="52"/>
+      <c r="H50" s="52"/>
+      <c r="I50" s="52"/>
+      <c r="J50" s="52"/>
+      <c r="K50" s="53"/>
+    </row>
+    <row r="51" spans="1:11" ht="24" customHeight="1">
+      <c r="A51" s="54"/>
+      <c r="B51" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E50" s="51"/>
-      <c r="F50" s="51"/>
-      <c r="G50" s="51"/>
-      <c r="H50" s="51"/>
-      <c r="I50" s="51"/>
-      <c r="J50" s="51"/>
-      <c r="K50" s="52"/>
-    </row>
-    <row r="51" spans="1:11" ht="24" customHeight="1">
-      <c r="A51" s="53"/>
-      <c r="B51" s="15" t="s">
+      <c r="C51" s="55"/>
+      <c r="D51" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C51" s="54"/>
-      <c r="D51" s="40" t="s">
+      <c r="E51" s="53"/>
+      <c r="F51" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E51" s="52"/>
-      <c r="F51" s="40" t="s">
+      <c r="G51" s="53"/>
+      <c r="H51" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="G51" s="52"/>
-      <c r="H51" s="41" t="s">
+      <c r="I51" s="53"/>
+      <c r="J51" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="52"/>
-      <c r="J51" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="K51" s="52"/>
+      <c r="K51" s="53"/>
     </row>
     <row r="52" spans="1:11" ht="24" customHeight="1">
-      <c r="A52" s="55"/>
+      <c r="A52" s="56"/>
       <c r="B52" s="19" t="str">
         <f>RUBRICA!A4</f>
         <v xml:space="preserve">1. Presenta el proyecto considerando la relevancia, objetivos, metodología y desarrollo, de acuerdo a los estándares de calidad de la disciplina. </v>
@@ -2513,19 +2508,19 @@
       </c>
       <c r="D52" s="12" t="str">
         <f t="shared" ref="D52:D56" si="17">IF($C52=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E52" s="12">
+        <v/>
+      </c>
+      <c r="E52" s="12" t="str">
         <f>IF(D52="X",100*0.15,"")</f>
-        <v>15</v>
+        <v/>
       </c>
       <c r="F52" s="12" t="str">
         <f t="shared" ref="F52:F56" si="18">IF($C52=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G52" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G52" s="12">
         <f>IF(F52="X",60*0.15,"")</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="H52" s="12" t="str">
         <f t="shared" ref="H52:H56" si="19">IF($C52=ML,"X","")</f>
@@ -2545,7 +2540,7 @@
       </c>
     </row>
     <row r="53" spans="1:11" ht="24" customHeight="1">
-      <c r="A53" s="55"/>
+      <c r="A53" s="56"/>
       <c r="B53" s="19" t="str">
         <f>RUBRICA!A5</f>
         <v xml:space="preserve">2. Presenta las evidencias del Proyecto APT, dando cuenta del cumplimiento de los objetivos y de acuerdo a los estándares de la disciplina. </v>
@@ -2555,19 +2550,19 @@
       </c>
       <c r="D53" s="12" t="str">
         <f t="shared" si="17"/>
-        <v>X</v>
-      </c>
-      <c r="E53" s="12">
+        <v/>
+      </c>
+      <c r="E53" s="12" t="str">
         <f>IF(D53="X",100*0.25,"")</f>
-        <v>25</v>
+        <v/>
       </c>
       <c r="F53" s="12" t="str">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="G53" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G53" s="12">
         <f>IF(F53="X",60*0.25,"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="H53" s="12" t="str">
         <f t="shared" si="19"/>
@@ -2587,7 +2582,7 @@
       </c>
     </row>
     <row r="54" spans="1:11" ht="24" customHeight="1">
-      <c r="A54" s="55"/>
+      <c r="A54" s="56"/>
       <c r="B54" s="19" t="str">
         <f>RUBRICA!A6</f>
         <v>3. Responde las preguntas realizadas por la comisión, cumpliendo con los estándares de calidad de la disciplina.</v>
@@ -2597,19 +2592,19 @@
       </c>
       <c r="D54" s="12" t="str">
         <f t="shared" si="17"/>
-        <v>X</v>
-      </c>
-      <c r="E54" s="12">
+        <v/>
+      </c>
+      <c r="E54" s="12" t="str">
         <f>IF(D54="X",100*0.2,"")</f>
-        <v>20</v>
+        <v/>
       </c>
       <c r="F54" s="12" t="str">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="G54" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G54" s="12">
         <f>IF(F54="X",60*0.2,"")</f>
-        <v/>
+        <v>12</v>
       </c>
       <c r="H54" s="12" t="str">
         <f t="shared" si="19"/>
@@ -2629,13 +2624,13 @@
       </c>
     </row>
     <row r="55" spans="1:11" ht="24" customHeight="1">
-      <c r="A55" s="55"/>
+      <c r="A55" s="56"/>
       <c r="B55" s="19" t="str">
         <f>RUBRICA!A7</f>
         <v>4. Expone el Proyecto APT, considerando el formato y el tiempo establecido para la presentación.</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D55" s="12" t="str">
         <f t="shared" si="17"/>
@@ -2671,7 +2666,7 @@
       </c>
     </row>
     <row r="56" spans="1:11" ht="24" customHeight="1">
-      <c r="A56" s="55"/>
+      <c r="A56" s="56"/>
       <c r="B56" s="19" t="str">
         <f>RUBRICA!A8</f>
         <v>5. Expresa sus ideas con fluidez, claridad y precisión, utilizando lenguaje técnico propio de la disciplina.</v>
@@ -2681,19 +2676,19 @@
       </c>
       <c r="D56" s="12" t="str">
         <f t="shared" si="17"/>
-        <v>X</v>
-      </c>
-      <c r="E56" s="12">
+        <v/>
+      </c>
+      <c r="E56" s="12" t="str">
         <f>IF(D56="X",100*0.05,"")</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="F56" s="12" t="str">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="G56" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G56" s="12">
         <f>IF(F56="X",60*0.05,"")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="H56" s="12" t="str">
         <f t="shared" si="19"/>
@@ -2713,13 +2708,13 @@
       </c>
     </row>
     <row r="57" spans="1:11" ht="24" customHeight="1">
-      <c r="A57" s="55"/>
+      <c r="A57" s="56"/>
       <c r="B57" s="19" t="str">
         <f>RUBRICA!A9</f>
         <v>6. Entrega la documentación y evidencias requerida por la asignatura de acuerdo a la estructura y nombres solicitados, guardando todas las evidencias de avances en Git</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D57" s="12" t="str">
         <f>IF($C57=CL,"X","")</f>
@@ -2755,7 +2750,7 @@
       </c>
     </row>
     <row r="58" spans="1:11" ht="24" customHeight="1">
-      <c r="A58" s="55"/>
+      <c r="A58" s="56"/>
       <c r="B58" s="19" t="str">
         <f>RUBRICA!A10</f>
         <v xml:space="preserve">7. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. </v>
@@ -2765,19 +2760,19 @@
       </c>
       <c r="D58" s="12" t="str">
         <f>IF($C58=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E58" s="12">
+        <v/>
+      </c>
+      <c r="E58" s="12" t="str">
         <f>IF(D58="X",100*0.1,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F58" s="12" t="str">
         <f>IF($C58=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G58" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G58" s="12">
         <f>IF(F58="X",60*0.1,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="H58" s="12" t="str">
         <f>IF($C58=ML,"X","")</f>
@@ -2797,23 +2792,23 @@
       </c>
     </row>
     <row r="59" spans="1:11" ht="24" customHeight="1">
-      <c r="A59" s="53"/>
+      <c r="A59" s="54"/>
       <c r="B59" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C59" s="22">
         <f>E59+G59+I59+K59</f>
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="D59" s="13"/>
       <c r="E59" s="13">
         <f>SUM(E52:E58)</f>
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F59" s="13"/>
       <c r="G59" s="13">
         <f>SUM(G52:G58)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="H59" s="13"/>
       <c r="I59" s="13">
@@ -2827,64 +2822,64 @@
       </c>
     </row>
     <row r="60" spans="1:11" ht="24" customHeight="1">
-      <c r="A60" s="54"/>
+      <c r="A60" s="55"/>
       <c r="B60" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C60" s="14">
         <f>VLOOKUP(C59,ESCALA_IEP!A41:B241,2,FALSE)</f>
-        <v>7</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="15.75" customHeight="1"/>
     <row r="62" spans="1:11" ht="15.75" customHeight="1"/>
     <row r="63" spans="1:11" ht="24" customHeight="1">
-      <c r="A63" s="42" t="s">
+      <c r="A63" s="39" t="s">
         <v>18</v>
       </c>
       <c r="B63" s="11" t="str">
         <f>B5</f>
-        <v>ESTUDIANTE 2</v>
-      </c>
-      <c r="C63" s="39" t="s">
+        <v>JOAN JARA</v>
+      </c>
+      <c r="C63" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D63" s="40" t="s">
+      <c r="E63" s="52"/>
+      <c r="F63" s="52"/>
+      <c r="G63" s="52"/>
+      <c r="H63" s="52"/>
+      <c r="I63" s="52"/>
+      <c r="J63" s="52"/>
+      <c r="K63" s="53"/>
+    </row>
+    <row r="64" spans="1:11" ht="24" customHeight="1">
+      <c r="A64" s="54"/>
+      <c r="B64" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E63" s="51"/>
-      <c r="F63" s="51"/>
-      <c r="G63" s="51"/>
-      <c r="H63" s="51"/>
-      <c r="I63" s="51"/>
-      <c r="J63" s="51"/>
-      <c r="K63" s="52"/>
-    </row>
-    <row r="64" spans="1:11" ht="24" customHeight="1">
-      <c r="A64" s="53"/>
-      <c r="B64" s="15" t="s">
+      <c r="C64" s="55"/>
+      <c r="D64" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C64" s="54"/>
-      <c r="D64" s="40" t="s">
+      <c r="E64" s="53"/>
+      <c r="F64" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E64" s="52"/>
-      <c r="F64" s="40" t="s">
+      <c r="G64" s="53"/>
+      <c r="H64" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="G64" s="52"/>
-      <c r="H64" s="41" t="s">
+      <c r="I64" s="53"/>
+      <c r="J64" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="I64" s="52"/>
-      <c r="J64" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="K64" s="52"/>
+      <c r="K64" s="53"/>
     </row>
     <row r="65" spans="1:11" ht="24" customHeight="1">
-      <c r="A65" s="55"/>
+      <c r="A65" s="56"/>
       <c r="B65" s="19" t="str">
         <f>RUBRICA!A4</f>
         <v xml:space="preserve">1. Presenta el proyecto considerando la relevancia, objetivos, metodología y desarrollo, de acuerdo a los estándares de calidad de la disciplina. </v>
@@ -2894,19 +2889,19 @@
       </c>
       <c r="D65" s="12" t="str">
         <f t="shared" ref="D65:D69" si="22">IF($C65=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E65" s="12">
+        <v/>
+      </c>
+      <c r="E65" s="12" t="str">
         <f>IF(D65="X",100*0.15,"")</f>
-        <v>15</v>
+        <v/>
       </c>
       <c r="F65" s="12" t="str">
         <f t="shared" ref="F65:F69" si="23">IF($C65=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G65" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G65" s="12">
         <f>IF(F65="X",60*0.15,"")</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="H65" s="12" t="str">
         <f t="shared" ref="H65:H69" si="24">IF($C65=ML,"X","")</f>
@@ -2926,7 +2921,7 @@
       </c>
     </row>
     <row r="66" spans="1:11" ht="24" customHeight="1">
-      <c r="A66" s="55"/>
+      <c r="A66" s="56"/>
       <c r="B66" s="19" t="str">
         <f>RUBRICA!A5</f>
         <v xml:space="preserve">2. Presenta las evidencias del Proyecto APT, dando cuenta del cumplimiento de los objetivos y de acuerdo a los estándares de la disciplina. </v>
@@ -2936,19 +2931,19 @@
       </c>
       <c r="D66" s="12" t="str">
         <f t="shared" si="22"/>
-        <v>X</v>
-      </c>
-      <c r="E66" s="12">
+        <v/>
+      </c>
+      <c r="E66" s="12" t="str">
         <f>IF(D66="X",100*0.25,"")</f>
-        <v>25</v>
+        <v/>
       </c>
       <c r="F66" s="12" t="str">
         <f t="shared" si="23"/>
-        <v/>
-      </c>
-      <c r="G66" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G66" s="12">
         <f>IF(F66="X",60*0.25,"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="H66" s="12" t="str">
         <f t="shared" si="24"/>
@@ -2968,21 +2963,21 @@
       </c>
     </row>
     <row r="67" spans="1:11" ht="24" customHeight="1">
-      <c r="A67" s="55"/>
+      <c r="A67" s="56"/>
       <c r="B67" s="19" t="str">
         <f>RUBRICA!A6</f>
         <v>3. Responde las preguntas realizadas por la comisión, cumpliendo con los estándares de calidad de la disciplina.</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D67" s="12" t="str">
         <f t="shared" si="22"/>
-        <v>X</v>
-      </c>
-      <c r="E67" s="12">
+        <v/>
+      </c>
+      <c r="E67" s="12" t="str">
         <f>IF(D67="X",100*0.2,"")</f>
-        <v>20</v>
+        <v/>
       </c>
       <c r="F67" s="12" t="str">
         <f t="shared" si="23"/>
@@ -2994,11 +2989,11 @@
       </c>
       <c r="H67" s="12" t="str">
         <f t="shared" si="24"/>
-        <v/>
-      </c>
-      <c r="I67" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="I67" s="12">
         <f>IF(H67="X",30*0.2,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="J67" s="12" t="str">
         <f t="shared" si="25"/>
@@ -3010,13 +3005,13 @@
       </c>
     </row>
     <row r="68" spans="1:11" ht="24" customHeight="1">
-      <c r="A68" s="55"/>
+      <c r="A68" s="56"/>
       <c r="B68" s="19" t="str">
         <f>RUBRICA!A7</f>
         <v>4. Expone el Proyecto APT, considerando el formato y el tiempo establecido para la presentación.</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D68" s="12" t="str">
         <f t="shared" si="22"/>
@@ -3052,21 +3047,21 @@
       </c>
     </row>
     <row r="69" spans="1:11" ht="24" customHeight="1">
-      <c r="A69" s="55"/>
+      <c r="A69" s="56"/>
       <c r="B69" s="19" t="str">
         <f>RUBRICA!A8</f>
         <v>5. Expresa sus ideas con fluidez, claridad y precisión, utilizando lenguaje técnico propio de la disciplina.</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D69" s="12" t="str">
         <f t="shared" si="22"/>
-        <v>X</v>
-      </c>
-      <c r="E69" s="12">
+        <v/>
+      </c>
+      <c r="E69" s="12" t="str">
         <f>IF(D69="X",100*0.05,"")</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="F69" s="12" t="str">
         <f t="shared" si="23"/>
@@ -3078,11 +3073,11 @@
       </c>
       <c r="H69" s="12" t="str">
         <f t="shared" si="24"/>
-        <v/>
-      </c>
-      <c r="I69" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="I69" s="12">
         <f>IF(H69="X",30*0.05,"")</f>
-        <v/>
+        <v>1.5</v>
       </c>
       <c r="J69" s="12" t="str">
         <f t="shared" si="25"/>
@@ -3094,13 +3089,13 @@
       </c>
     </row>
     <row r="70" spans="1:11" ht="24" customHeight="1">
-      <c r="A70" s="55"/>
+      <c r="A70" s="56"/>
       <c r="B70" s="19" t="str">
         <f>RUBRICA!A9</f>
         <v>6. Entrega la documentación y evidencias requerida por la asignatura de acuerdo a la estructura y nombres solicitados, guardando todas las evidencias de avances en Git</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D70" s="12" t="str">
         <f>IF($C70=CL,"X","")</f>
@@ -3136,7 +3131,7 @@
       </c>
     </row>
     <row r="71" spans="1:11" ht="24" customHeight="1">
-      <c r="A71" s="55"/>
+      <c r="A71" s="56"/>
       <c r="B71" s="19" t="str">
         <f>RUBRICA!A10</f>
         <v xml:space="preserve">7. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. </v>
@@ -3146,19 +3141,19 @@
       </c>
       <c r="D71" s="12" t="str">
         <f>IF($C71=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E71" s="12">
+        <v/>
+      </c>
+      <c r="E71" s="12" t="str">
         <f>IF(D71="X",100*0.1,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F71" s="12" t="str">
         <f>IF($C71=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G71" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G71" s="12">
         <f>IF(F71="X",60*0.1,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="H71" s="12" t="str">
         <f>IF($C71=ML,"X","")</f>
@@ -3178,28 +3173,28 @@
       </c>
     </row>
     <row r="72" spans="1:11" ht="24" customHeight="1">
-      <c r="A72" s="53"/>
+      <c r="A72" s="54"/>
       <c r="B72" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C72" s="22">
         <f>E72+G72+I72+K72</f>
-        <v>100</v>
+        <v>62.5</v>
       </c>
       <c r="D72" s="13"/>
       <c r="E72" s="13">
         <f>SUM(E65:E71)</f>
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F72" s="13"/>
       <c r="G72" s="13">
         <f>SUM(G65:G71)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H72" s="13"/>
       <c r="I72" s="13">
         <f>SUM(I65:I71)</f>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="J72" s="13"/>
       <c r="K72" s="13">
@@ -3208,70 +3203,70 @@
       </c>
     </row>
     <row r="73" spans="1:11" ht="24" customHeight="1">
-      <c r="A73" s="54"/>
+      <c r="A73" s="55"/>
       <c r="B73" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C73" s="14">
         <f>VLOOKUP(C72,ESCALA_IEP!A54:B254,2,FALSE)</f>
-        <v>7</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="74" spans="1:11" ht="15.75" customHeight="1"/>
     <row r="75" spans="1:11" ht="15.75" customHeight="1"/>
     <row r="76" spans="1:11" ht="24" customHeight="1">
-      <c r="A76" s="42" t="s">
+      <c r="A76" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B76" s="11" t="str">
+      <c r="B76" s="11">
         <f>B6</f>
-        <v>ESTUDIANTE 3</v>
-      </c>
-      <c r="C76" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D76" s="40" t="s">
+      <c r="E76" s="52"/>
+      <c r="F76" s="52"/>
+      <c r="G76" s="52"/>
+      <c r="H76" s="52"/>
+      <c r="I76" s="52"/>
+      <c r="J76" s="52"/>
+      <c r="K76" s="53"/>
+    </row>
+    <row r="77" spans="1:11" ht="24" customHeight="1">
+      <c r="A77" s="54"/>
+      <c r="B77" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E76" s="51"/>
-      <c r="F76" s="51"/>
-      <c r="G76" s="51"/>
-      <c r="H76" s="51"/>
-      <c r="I76" s="51"/>
-      <c r="J76" s="51"/>
-      <c r="K76" s="52"/>
-    </row>
-    <row r="77" spans="1:11" ht="24" customHeight="1">
-      <c r="A77" s="53"/>
-      <c r="B77" s="15" t="s">
+      <c r="C77" s="55"/>
+      <c r="D77" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C77" s="54"/>
-      <c r="D77" s="40" t="s">
+      <c r="E77" s="53"/>
+      <c r="F77" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E77" s="52"/>
-      <c r="F77" s="40" t="s">
+      <c r="G77" s="53"/>
+      <c r="H77" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="G77" s="52"/>
-      <c r="H77" s="41" t="s">
+      <c r="I77" s="53"/>
+      <c r="J77" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="I77" s="52"/>
-      <c r="J77" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="K77" s="52"/>
+      <c r="K77" s="53"/>
     </row>
     <row r="78" spans="1:11" ht="24" customHeight="1">
-      <c r="A78" s="55"/>
+      <c r="A78" s="56"/>
       <c r="B78" s="19" t="str">
         <f>RUBRICA!A4</f>
         <v xml:space="preserve">1. Presenta el proyecto considerando la relevancia, objetivos, metodología y desarrollo, de acuerdo a los estándares de calidad de la disciplina. </v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D78" s="12" t="str">
         <f t="shared" ref="D78:D82" si="27">IF($C78=CL,"X","")</f>
@@ -3307,7 +3302,7 @@
       </c>
     </row>
     <row r="79" spans="1:11" ht="24" customHeight="1">
-      <c r="A79" s="55"/>
+      <c r="A79" s="56"/>
       <c r="B79" s="19" t="str">
         <f>RUBRICA!A5</f>
         <v xml:space="preserve">2. Presenta las evidencias del Proyecto APT, dando cuenta del cumplimiento de los objetivos y de acuerdo a los estándares de la disciplina. </v>
@@ -3317,19 +3312,19 @@
       </c>
       <c r="D79" s="12" t="str">
         <f t="shared" si="27"/>
-        <v>X</v>
-      </c>
-      <c r="E79" s="12">
+        <v/>
+      </c>
+      <c r="E79" s="12" t="str">
         <f>IF(D79="X",100*0.25,"")</f>
-        <v>25</v>
+        <v/>
       </c>
       <c r="F79" s="12" t="str">
         <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="G79" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G79" s="12">
         <f>IF(F79="X",60*0.25,"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="H79" s="12" t="str">
         <f t="shared" si="29"/>
@@ -3349,7 +3344,7 @@
       </c>
     </row>
     <row r="80" spans="1:11" ht="24" customHeight="1">
-      <c r="A80" s="55"/>
+      <c r="A80" s="56"/>
       <c r="B80" s="19" t="str">
         <f>RUBRICA!A6</f>
         <v>3. Responde las preguntas realizadas por la comisión, cumpliendo con los estándares de calidad de la disciplina.</v>
@@ -3359,19 +3354,19 @@
       </c>
       <c r="D80" s="12" t="str">
         <f t="shared" si="27"/>
-        <v>X</v>
-      </c>
-      <c r="E80" s="12">
+        <v/>
+      </c>
+      <c r="E80" s="12" t="str">
         <f>IF(D80="X",100*0.2,"")</f>
-        <v>20</v>
+        <v/>
       </c>
       <c r="F80" s="12" t="str">
         <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="G80" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G80" s="12">
         <f>IF(F80="X",60*0.2,"")</f>
-        <v/>
+        <v>12</v>
       </c>
       <c r="H80" s="12" t="str">
         <f t="shared" si="29"/>
@@ -3391,13 +3386,13 @@
       </c>
     </row>
     <row r="81" spans="1:11" ht="24" customHeight="1">
-      <c r="A81" s="55"/>
+      <c r="A81" s="56"/>
       <c r="B81" s="19" t="str">
         <f>RUBRICA!A7</f>
         <v>4. Expone el Proyecto APT, considerando el formato y el tiempo establecido para la presentación.</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D81" s="12" t="str">
         <f t="shared" si="27"/>
@@ -3433,7 +3428,7 @@
       </c>
     </row>
     <row r="82" spans="1:11" ht="24" customHeight="1">
-      <c r="A82" s="55"/>
+      <c r="A82" s="56"/>
       <c r="B82" s="19" t="str">
         <f>RUBRICA!A8</f>
         <v>5. Expresa sus ideas con fluidez, claridad y precisión, utilizando lenguaje técnico propio de la disciplina.</v>
@@ -3443,19 +3438,19 @@
       </c>
       <c r="D82" s="12" t="str">
         <f t="shared" si="27"/>
-        <v>X</v>
-      </c>
-      <c r="E82" s="12">
+        <v/>
+      </c>
+      <c r="E82" s="12" t="str">
         <f>IF(D82="X",100*0.05,"")</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="F82" s="12" t="str">
         <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="G82" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G82" s="12">
         <f>IF(F82="X",60*0.05,"")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="H82" s="12" t="str">
         <f t="shared" si="29"/>
@@ -3475,13 +3470,13 @@
       </c>
     </row>
     <row r="83" spans="1:11" ht="24" customHeight="1">
-      <c r="A83" s="55"/>
+      <c r="A83" s="56"/>
       <c r="B83" s="19" t="str">
         <f>RUBRICA!A9</f>
         <v>6. Entrega la documentación y evidencias requerida por la asignatura de acuerdo a la estructura y nombres solicitados, guardando todas las evidencias de avances en Git</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D83" s="12" t="str">
         <f>IF($C83=CL,"X","")</f>
@@ -3517,7 +3512,7 @@
       </c>
     </row>
     <row r="84" spans="1:11" ht="24" customHeight="1">
-      <c r="A84" s="55"/>
+      <c r="A84" s="56"/>
       <c r="B84" s="19" t="str">
         <f>RUBRICA!A10</f>
         <v xml:space="preserve">7. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. </v>
@@ -3527,19 +3522,19 @@
       </c>
       <c r="D84" s="12" t="str">
         <f>IF($C84=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E84" s="12">
+        <v/>
+      </c>
+      <c r="E84" s="12" t="str">
         <f>IF(D84="X",100*0.1,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F84" s="12" t="str">
         <f>IF($C84=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G84" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G84" s="12">
         <f>IF(F84="X",60*0.1,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="H84" s="12" t="str">
         <f>IF($C84=ML,"X","")</f>
@@ -3559,23 +3554,23 @@
       </c>
     </row>
     <row r="85" spans="1:11" ht="24" customHeight="1">
-      <c r="A85" s="53"/>
+      <c r="A85" s="54"/>
       <c r="B85" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C85" s="22">
         <f>E85+G85+I85+K85</f>
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="D85" s="13"/>
       <c r="E85" s="13">
         <f>SUM(E78:E84)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="F85" s="13"/>
       <c r="G85" s="13">
         <f>SUM(G78:G84)</f>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="H85" s="13"/>
       <c r="I85" s="13">
@@ -3589,13 +3584,13 @@
       </c>
     </row>
     <row r="86" spans="1:11" ht="24" customHeight="1">
-      <c r="A86" s="54"/>
+      <c r="A86" s="55"/>
       <c r="B86" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C86" s="14">
         <f>VLOOKUP(C85,ESCALA_IEP!A67:B267,2,FALSE)</f>
-        <v>7</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="87" spans="1:11" ht="15.75" customHeight="1"/>
@@ -4311,32 +4306,6 @@
     <row r="797" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="A76:A86"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="D76:K76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="J77:K77"/>
-    <mergeCell ref="A63:A73"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="D63:K63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="D24:K24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="A50:A60"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:K50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="J51:K51"/>
     <mergeCell ref="A11:A21"/>
     <mergeCell ref="C37:C38"/>
     <mergeCell ref="D37:K37"/>
@@ -4353,6 +4322,32 @@
     <mergeCell ref="A37:A47"/>
     <mergeCell ref="A24:A34"/>
     <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A50:A60"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:K50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="D24:K24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="A63:A73"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="D63:K63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="A76:A86"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="D76:K76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="J77:K77"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:C6">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
@@ -4404,46 +4399,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="43" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="44" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="44"/>
-      <c r="B2" s="48" t="s">
+      <c r="A2" s="45"/>
+      <c r="B2" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="49" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="25" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="44"/>
+        <v>13</v>
+      </c>
+      <c r="F2" s="45"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="44"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
       <c r="D3" s="27">
         <v>0.3</v>
       </c>
       <c r="E3" s="27">
         <v>0</v>
       </c>
-      <c r="F3" s="44"/>
+      <c r="F3" s="45"/>
     </row>
     <row r="4" spans="1:6" ht="110.45">
       <c r="A4" s="23" t="s">
@@ -4612,10 +4607,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="14.45">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.45">
@@ -8440,10 +8435,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="14.45">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.45">
@@ -9756,34 +9751,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.45">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>63</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" ht="43.9" thickBot="1">
-      <c r="A2" s="56"/>
+      <c r="A2" s="57"/>
       <c r="B2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="57" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29.45" thickBot="1">
       <c r="A3" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="10">
         <v>4</v>

</xml_diff>